<commit_message>
adição de algumas informações
</commit_message>
<xml_diff>
--- a/2025 - PLANILHA CONTROLE SCOMP-2025.xlsx
+++ b/2025 - PLANILHA CONTROLE SCOMP-2025.xlsx
@@ -531,48 +531,43 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>45735</v>
+        <v>45565</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>44555666777</t>
+          <t>SEI-260007/016010/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SLA</t>
+          <t>DIVLS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sdasd</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>hjhjh</t>
+          <t>Licitação</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>fulano</t>
+          <t>Maria Eduarda</t>
         </is>
       </c>
       <c r="H2" s="3" t="n">
-        <v>45721</v>
+        <v>45565</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4344543</t>
+          <t>10034/2024</t>
         </is>
       </c>
       <c r="J2" s="3" t="n">
-        <v>45693</v>
+        <v>45666</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>45735</v>
@@ -583,27 +578,27 @@
         </is>
       </c>
       <c r="M2" s="3" t="n">
-        <v>45703</v>
+        <v>45667</v>
       </c>
       <c r="N2" t="n">
-        <v>-32</v>
+        <v>102</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>September</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>365</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Saiu em 15/02/2025</t>
+          <t>Saiu em 10/01/2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
subindo commit com banco de dados
</commit_message>
<xml_diff>
--- a/2025 - PLANILHA CONTROLE SCOMP-2025.xlsx
+++ b/2025 - PLANILHA CONTROLE SCOMP-2025.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,11 +523,6 @@
           <t>Contador Total</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Observação</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
@@ -535,12 +530,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SEI-260007/016010/2024</t>
+          <t>SEI-260007/005119/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DIVLS</t>
+          <t>OPMES</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -550,24 +545,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Maria Eduarda</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="n">
+          <t>Robson</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>8046/2024</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="n">
         <v>45565</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>10034/2024</t>
-        </is>
-      </c>
-      <c r="J2" s="3" t="n">
-        <v>45666</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>45735</v>
@@ -585,21 +577,16 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>Janeiro</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>8</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>365</v>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Saiu em 10/01/2025</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>